<commit_message>
Updated text about Jytte Strøm
</commit_message>
<xml_diff>
--- a/Admin/MetatekstV3.xlsx
+++ b/Admin/MetatekstV3.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="72">
   <si>
     <t>Økologisk pil til kurveflet eller levende hegn, vælg imellem mange farver og tykkelser</t>
   </si>
@@ -209,9 +209,6 @@
     <t>Titel (vises øverst på side og som overskrift i søgemaskine) max 70 tegn</t>
   </si>
   <si>
-    <t>Tekst (vises kun i søgemaskine) max 155 tegn</t>
-  </si>
-  <si>
     <t>Tekst (vises kun  i søgemaskine) max 155 tegn</t>
   </si>
   <si>
@@ -228,6 +225,12 @@
   </si>
   <si>
     <t>Peter: oversætte</t>
+  </si>
+  <si>
+    <t>Titel (vises øverst på side og som overskrift i søgemaskine) max 70 tegn &lt;title&gt;</t>
+  </si>
+  <si>
+    <t>Tekst (vises kun i søgemaskine) max 155 tegn  &lt;meta name="description" content="xxx"/&gt;</t>
   </si>
 </sst>
 </file>
@@ -398,7 +401,7 @@
     <cellStyle name="Neutral" xfId="1" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="14">
+  <dxfs count="13">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -506,16 +509,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -842,7 +835,7 @@
   <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -857,10 +850,10 @@
   <sheetData>
     <row r="1" spans="1:10" s="15" customFormat="1" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D1" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="E1" s="15" t="s">
         <v>68</v>
-      </c>
-      <c r="E1" s="15" t="s">
-        <v>69</v>
       </c>
       <c r="F1" s="16"/>
       <c r="G1" s="16"/>
@@ -876,10 +869,10 @@
         <v>2</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
       <c r="F2" s="13" t="s">
         <v>61</v>
@@ -976,7 +969,7 @@
         <v>53</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F5" s="10">
         <f t="shared" ref="F5:G15" si="1">LEN(D5)</f>
@@ -1224,7 +1217,7 @@
         <v>27</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F13" s="10">
         <f t="shared" si="1"/>
@@ -1335,6 +1328,7 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1357,16 +1351,16 @@
   <sheetData>
     <row r="1" spans="1:9" s="15" customFormat="1" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" s="15" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C1" s="15" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D1" s="15" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E1" s="15" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="2" spans="1:9" s="14" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -1383,7 +1377,7 @@
         <v>63</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F2" s="13" t="s">
         <v>61</v>
@@ -1474,7 +1468,7 @@
         <v>53</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F5" s="10">
         <f t="shared" ref="F5:G15" si="1">LEN(D5)</f>
@@ -1722,7 +1716,7 @@
         <v>27</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F13" s="10">
         <f t="shared" si="1"/>

</xml_diff>